<commit_message>
MTR402 TC-36497 MTR-138 TC-38492 added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SCHO3.xlsx
+++ b/src/test/resources/testdata/SCHO3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\git\AutomationCucumber2023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27325EE7-4780-4A5C-B41E-36E2F982CD59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCF417C-819F-45BF-8C7A-6BE7466E53C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="19416" windowHeight="10416" xr2:uid="{CD3A54CB-C005-0E4A-932C-421D6A132F4C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>FirstName</t>
   </si>
@@ -108,9 +108,6 @@
     <t>29418</t>
   </si>
   <si>
-    <t>08152023</t>
-  </si>
-  <si>
     <t>South Carolina</t>
   </si>
   <si>
@@ -130,6 +127,12 @@
   </si>
   <si>
     <t>Richards</t>
+  </si>
+  <si>
+    <t>09212023</t>
+  </si>
+  <si>
+    <t>2023</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -580,10 +583,10 @@
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -595,16 +598,16 @@
         <v>26</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>18</v>
@@ -618,11 +621,11 @@
       <c r="M2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="6">
-        <v>2022</v>
+      <c r="N2" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>23</v>
@@ -630,10 +633,10 @@
     </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -645,16 +648,16 @@
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>19</v>
@@ -668,11 +671,11 @@
       <c r="M3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="6">
-        <v>2022</v>
+      <c r="N3" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>24</v>

</xml_diff>